<commit_message>
Added - Multiprocessing - More Table Data - Table Plot
</commit_message>
<xml_diff>
--- a/plots/database.xlsx
+++ b/plots/database.xlsx
@@ -11,6 +11,8 @@
     <sheet name="lowcost" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="bestratio" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="t_highsuccess" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="t_lowcost" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="t_bestratio" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -428,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G214"/>
+  <dimension ref="A1:G229"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6643,6 +6645,441 @@
       </c>
       <c r="G214" t="n">
         <v>0.0157</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="1" t="n">
+        <v>213</v>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="E215" t="n">
+        <v>0.8130775889826612</v>
+      </c>
+      <c r="F215" t="n">
+        <v>66.0751840948701</v>
+      </c>
+      <c r="G215" t="n">
+        <v>0.0123</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>URC</t>
+        </is>
+      </c>
+      <c r="E216" t="n">
+        <v>0.862</v>
+      </c>
+      <c r="F216" t="n">
+        <v>63.334</v>
+      </c>
+      <c r="G216" t="n">
+        <v>0.0136</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="1" t="n">
+        <v>215</v>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>URC Mod</t>
+        </is>
+      </c>
+      <c r="E217" t="n">
+        <v>0.853</v>
+      </c>
+      <c r="F217" t="n">
+        <v>63.139</v>
+      </c>
+      <c r="G217" t="n">
+        <v>0.0135</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="E218" t="n">
+        <v>0.8033408729231484</v>
+      </c>
+      <c r="F218" t="n">
+        <v>65.34044816202186</v>
+      </c>
+      <c r="G218" t="n">
+        <v>0.0123</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="1" t="n">
+        <v>217</v>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>URC</t>
+        </is>
+      </c>
+      <c r="E219" t="n">
+        <v>0.846</v>
+      </c>
+      <c r="F219" t="n">
+        <v>58.199</v>
+      </c>
+      <c r="G219" t="n">
+        <v>0.0145</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="1" t="n">
+        <v>218</v>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>URC Mod</t>
+        </is>
+      </c>
+      <c r="E220" t="n">
+        <v>0.846</v>
+      </c>
+      <c r="F220" t="n">
+        <v>58.056</v>
+      </c>
+      <c r="G220" t="n">
+        <v>0.0146</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="1" t="n">
+        <v>219</v>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="E221" t="n">
+        <v>0.799583552906183</v>
+      </c>
+      <c r="F221" t="n">
+        <v>64.7889690972419</v>
+      </c>
+      <c r="G221" t="n">
+        <v>0.0123</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="1" t="n">
+        <v>220</v>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>URC</t>
+        </is>
+      </c>
+      <c r="E222" t="n">
+        <v>0.819</v>
+      </c>
+      <c r="F222" t="n">
+        <v>61.14</v>
+      </c>
+      <c r="G222" t="n">
+        <v>0.0134</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="1" t="n">
+        <v>221</v>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>URC Mod</t>
+        </is>
+      </c>
+      <c r="E223" t="n">
+        <v>0.8120000000000001</v>
+      </c>
+      <c r="F223" t="n">
+        <v>60.196</v>
+      </c>
+      <c r="G223" t="n">
+        <v>0.0135</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="1" t="n">
+        <v>222</v>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="E224" t="n">
+        <v>0.8888255845594862</v>
+      </c>
+      <c r="F224" t="n">
+        <v>62.40148225547854</v>
+      </c>
+      <c r="G224" t="n">
+        <v>0.0142</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="1" t="n">
+        <v>223</v>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>URC</t>
+        </is>
+      </c>
+      <c r="E225" t="n">
+        <v>0.917</v>
+      </c>
+      <c r="F225" t="n">
+        <v>68.31</v>
+      </c>
+      <c r="G225" t="n">
+        <v>0.0134</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="1" t="n">
+        <v>224</v>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>URC Mod</t>
+        </is>
+      </c>
+      <c r="E226" t="n">
+        <v>0.909</v>
+      </c>
+      <c r="F226" t="n">
+        <v>68.01600000000001</v>
+      </c>
+      <c r="G226" t="n">
+        <v>0.0134</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="1" t="n">
+        <v>225</v>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="E227" t="n">
+        <v>0.862429144490119</v>
+      </c>
+      <c r="F227" t="n">
+        <v>60.99413003013393</v>
+      </c>
+      <c r="G227" t="n">
+        <v>0.0141</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="1" t="n">
+        <v>226</v>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>URC</t>
+        </is>
+      </c>
+      <c r="E228" t="n">
+        <v>0.899</v>
+      </c>
+      <c r="F228" t="n">
+        <v>62.76</v>
+      </c>
+      <c r="G228" t="n">
+        <v>0.0143</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="1" t="n">
+        <v>227</v>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>URC Mod</t>
+        </is>
+      </c>
+      <c r="E229" t="n">
+        <v>0.882</v>
+      </c>
+      <c r="F229" t="n">
+        <v>57.563</v>
+      </c>
+      <c r="G229" t="n">
+        <v>0.0153</v>
       </c>
     </row>
   </sheetData>
@@ -6656,7 +7093,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G214"/>
+  <dimension ref="A1:G229"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12867,6 +13304,441 @@
       </c>
       <c r="G214" t="n">
         <v>0.0323</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="1" t="n">
+        <v>213</v>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="E215" t="n">
+        <v>0.567889216676512</v>
+      </c>
+      <c r="F215" t="n">
+        <v>20.52368151679491</v>
+      </c>
+      <c r="G215" t="n">
+        <v>0.0277</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>URC</t>
+        </is>
+      </c>
+      <c r="E216" t="n">
+        <v>0.581</v>
+      </c>
+      <c r="F216" t="n">
+        <v>24.82</v>
+      </c>
+      <c r="G216" t="n">
+        <v>0.0234</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="1" t="n">
+        <v>215</v>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>URC Mod</t>
+        </is>
+      </c>
+      <c r="E217" t="n">
+        <v>0.608</v>
+      </c>
+      <c r="F217" t="n">
+        <v>24.461</v>
+      </c>
+      <c r="G217" t="n">
+        <v>0.0249</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="E218" t="n">
+        <v>0.5669286253445531</v>
+      </c>
+      <c r="F218" t="n">
+        <v>20.55736320329397</v>
+      </c>
+      <c r="G218" t="n">
+        <v>0.0276</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="1" t="n">
+        <v>217</v>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>URC</t>
+        </is>
+      </c>
+      <c r="E219" t="n">
+        <v>0.681</v>
+      </c>
+      <c r="F219" t="n">
+        <v>27.011</v>
+      </c>
+      <c r="G219" t="n">
+        <v>0.0252</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="1" t="n">
+        <v>218</v>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>URC Mod</t>
+        </is>
+      </c>
+      <c r="E220" t="n">
+        <v>0.588</v>
+      </c>
+      <c r="F220" t="n">
+        <v>24.365</v>
+      </c>
+      <c r="G220" t="n">
+        <v>0.0241</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="1" t="n">
+        <v>219</v>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="E221" t="n">
+        <v>0.5895699936597699</v>
+      </c>
+      <c r="F221" t="n">
+        <v>20.78735236007471</v>
+      </c>
+      <c r="G221" t="n">
+        <v>0.0284</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="1" t="n">
+        <v>220</v>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>URC</t>
+        </is>
+      </c>
+      <c r="E222" t="n">
+        <v>0.617</v>
+      </c>
+      <c r="F222" t="n">
+        <v>23.932</v>
+      </c>
+      <c r="G222" t="n">
+        <v>0.0258</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="1" t="n">
+        <v>221</v>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>URC Mod</t>
+        </is>
+      </c>
+      <c r="E223" t="n">
+        <v>0.624</v>
+      </c>
+      <c r="F223" t="n">
+        <v>23.75</v>
+      </c>
+      <c r="G223" t="n">
+        <v>0.0263</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="1" t="n">
+        <v>222</v>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="E224" t="n">
+        <v>0.6405954066749788</v>
+      </c>
+      <c r="F224" t="n">
+        <v>19.86454379335952</v>
+      </c>
+      <c r="G224" t="n">
+        <v>0.0322</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="1" t="n">
+        <v>223</v>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>URC</t>
+        </is>
+      </c>
+      <c r="E225" t="n">
+        <v>0.645</v>
+      </c>
+      <c r="F225" t="n">
+        <v>20.28</v>
+      </c>
+      <c r="G225" t="n">
+        <v>0.0318</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="1" t="n">
+        <v>224</v>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>URC Mod</t>
+        </is>
+      </c>
+      <c r="E226" t="n">
+        <v>0.626</v>
+      </c>
+      <c r="F226" t="n">
+        <v>20.151</v>
+      </c>
+      <c r="G226" t="n">
+        <v>0.0311</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="1" t="n">
+        <v>225</v>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="E227" t="n">
+        <v>0.5998333137485583</v>
+      </c>
+      <c r="F227" t="n">
+        <v>19.30982057712849</v>
+      </c>
+      <c r="G227" t="n">
+        <v>0.0311</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="1" t="n">
+        <v>226</v>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>URC</t>
+        </is>
+      </c>
+      <c r="E228" t="n">
+        <v>0.665</v>
+      </c>
+      <c r="F228" t="n">
+        <v>23.588</v>
+      </c>
+      <c r="G228" t="n">
+        <v>0.0282</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="1" t="n">
+        <v>227</v>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>URC Mod</t>
+        </is>
+      </c>
+      <c r="E229" t="n">
+        <v>0.611</v>
+      </c>
+      <c r="F229" t="n">
+        <v>19.975</v>
+      </c>
+      <c r="G229" t="n">
+        <v>0.0306</v>
       </c>
     </row>
   </sheetData>
@@ -12880,7 +13752,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G214"/>
+  <dimension ref="A1:G229"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19095,6 +19967,441 @@
       </c>
       <c r="G214" t="n">
         <v>0.0323</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="1" t="n">
+        <v>213</v>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="E215" t="n">
+        <v>0.567889216676512</v>
+      </c>
+      <c r="F215" t="n">
+        <v>20.52368151679491</v>
+      </c>
+      <c r="G215" t="n">
+        <v>0.0277</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>URC</t>
+        </is>
+      </c>
+      <c r="E216" t="n">
+        <v>0.707</v>
+      </c>
+      <c r="F216" t="n">
+        <v>27.853</v>
+      </c>
+      <c r="G216" t="n">
+        <v>0.0254</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="1" t="n">
+        <v>215</v>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>URC Mod</t>
+        </is>
+      </c>
+      <c r="E217" t="n">
+        <v>0.6830000000000001</v>
+      </c>
+      <c r="F217" t="n">
+        <v>26.364</v>
+      </c>
+      <c r="G217" t="n">
+        <v>0.0259</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="E218" t="n">
+        <v>0.5669286253445531</v>
+      </c>
+      <c r="F218" t="n">
+        <v>20.55736320329397</v>
+      </c>
+      <c r="G218" t="n">
+        <v>0.0276</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="1" t="n">
+        <v>217</v>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>URC</t>
+        </is>
+      </c>
+      <c r="E219" t="n">
+        <v>0.745</v>
+      </c>
+      <c r="F219" t="n">
+        <v>27.608</v>
+      </c>
+      <c r="G219" t="n">
+        <v>0.027</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="1" t="n">
+        <v>218</v>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>URC Mod</t>
+        </is>
+      </c>
+      <c r="E220" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F220" t="n">
+        <v>27.671</v>
+      </c>
+      <c r="G220" t="n">
+        <v>0.0271</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="1" t="n">
+        <v>219</v>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="E221" t="n">
+        <v>0.5895699936597699</v>
+      </c>
+      <c r="F221" t="n">
+        <v>20.78735236007471</v>
+      </c>
+      <c r="G221" t="n">
+        <v>0.0284</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="1" t="n">
+        <v>220</v>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>URC</t>
+        </is>
+      </c>
+      <c r="E222" t="n">
+        <v>0.626</v>
+      </c>
+      <c r="F222" t="n">
+        <v>24.012</v>
+      </c>
+      <c r="G222" t="n">
+        <v>0.0261</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="1" t="n">
+        <v>221</v>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>URC Mod</t>
+        </is>
+      </c>
+      <c r="E223" t="n">
+        <v>0.624</v>
+      </c>
+      <c r="F223" t="n">
+        <v>23.75</v>
+      </c>
+      <c r="G223" t="n">
+        <v>0.0263</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="1" t="n">
+        <v>222</v>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="E224" t="n">
+        <v>0.6405954066749788</v>
+      </c>
+      <c r="F224" t="n">
+        <v>19.86454379335952</v>
+      </c>
+      <c r="G224" t="n">
+        <v>0.0322</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="1" t="n">
+        <v>223</v>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>URC</t>
+        </is>
+      </c>
+      <c r="E225" t="n">
+        <v>0.645</v>
+      </c>
+      <c r="F225" t="n">
+        <v>20.28</v>
+      </c>
+      <c r="G225" t="n">
+        <v>0.0318</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="1" t="n">
+        <v>224</v>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>URC Mod</t>
+        </is>
+      </c>
+      <c r="E226" t="n">
+        <v>0.644</v>
+      </c>
+      <c r="F226" t="n">
+        <v>20.223</v>
+      </c>
+      <c r="G226" t="n">
+        <v>0.0318</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="1" t="n">
+        <v>225</v>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="E227" t="n">
+        <v>0.5998333137485583</v>
+      </c>
+      <c r="F227" t="n">
+        <v>19.30982057712849</v>
+      </c>
+      <c r="G227" t="n">
+        <v>0.0311</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="1" t="n">
+        <v>226</v>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>URC</t>
+        </is>
+      </c>
+      <c r="E228" t="n">
+        <v>0.777</v>
+      </c>
+      <c r="F228" t="n">
+        <v>26.506</v>
+      </c>
+      <c r="G228" t="n">
+        <v>0.0293</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="1" t="n">
+        <v>227</v>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>URC Mod</t>
+        </is>
+      </c>
+      <c r="E229" t="n">
+        <v>0.611</v>
+      </c>
+      <c r="F229" t="n">
+        <v>19.975</v>
+      </c>
+      <c r="G229" t="n">
+        <v>0.0306</v>
       </c>
     </row>
   </sheetData>
@@ -19108,7 +20415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19152,6 +20459,21 @@
           <t>Baseline Percentage</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>URC Cum. Percentage</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>URC Mod Cum. Percentage</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Baseline Cum. Percentage</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -19160,23 +20482,32 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C2" t="n">
         <v>7</v>
       </c>
       <c r="D2" t="n">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="E2" t="n">
-        <v>22.54</v>
+        <v>23.68</v>
       </c>
       <c r="F2" t="n">
-        <v>9.859999999999999</v>
+        <v>9.210000000000001</v>
       </c>
       <c r="G2" t="n">
         <v>100</v>
       </c>
+      <c r="H2" t="n">
+        <v>23.68</v>
+      </c>
+      <c r="I2" t="n">
+        <v>9.210000000000001</v>
+      </c>
+      <c r="J2" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -19194,14 +20525,23 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>12.68</v>
+        <v>11.84</v>
       </c>
       <c r="F3" t="n">
-        <v>16.9</v>
+        <v>15.79</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
       </c>
+      <c r="H3" t="n">
+        <v>35.52</v>
+      </c>
+      <c r="I3" t="n">
+        <v>25</v>
+      </c>
+      <c r="J3" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -19210,23 +20550,32 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>7.04</v>
+        <v>7.89</v>
       </c>
       <c r="F4" t="n">
-        <v>9.859999999999999</v>
+        <v>10.53</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
       </c>
+      <c r="H4" t="n">
+        <v>43.41</v>
+      </c>
+      <c r="I4" t="n">
+        <v>35.53</v>
+      </c>
+      <c r="J4" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -19238,20 +20587,29 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>5.63</v>
+        <v>5.26</v>
       </c>
       <c r="F5" t="n">
-        <v>15.49</v>
+        <v>18.42</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
       </c>
+      <c r="H5" t="n">
+        <v>48.66999999999999</v>
+      </c>
+      <c r="I5" t="n">
+        <v>53.95</v>
+      </c>
+      <c r="J5" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -19263,20 +20621,29 @@
         <v>7</v>
       </c>
       <c r="C6" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>9.859999999999999</v>
+        <v>9.210000000000001</v>
       </c>
       <c r="F6" t="n">
-        <v>11.27</v>
+        <v>11.84</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
       </c>
+      <c r="H6" t="n">
+        <v>57.88</v>
+      </c>
+      <c r="I6" t="n">
+        <v>65.79000000000001</v>
+      </c>
+      <c r="J6" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -19294,14 +20661,23 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>9.859999999999999</v>
+        <v>9.210000000000001</v>
       </c>
       <c r="F7" t="n">
-        <v>8.449999999999999</v>
+        <v>7.89</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
+      <c r="H7" t="n">
+        <v>67.09</v>
+      </c>
+      <c r="I7" t="n">
+        <v>73.68000000000001</v>
+      </c>
+      <c r="J7" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -19319,14 +20695,23 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>7.04</v>
+        <v>6.58</v>
       </c>
       <c r="F8" t="n">
-        <v>9.859999999999999</v>
+        <v>9.210000000000001</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
+      <c r="H8" t="n">
+        <v>73.67</v>
+      </c>
+      <c r="I8" t="n">
+        <v>82.89000000000001</v>
+      </c>
+      <c r="J8" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -19344,14 +20729,23 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>9.859999999999999</v>
+        <v>9.210000000000001</v>
       </c>
       <c r="F9" t="n">
-        <v>5.63</v>
+        <v>5.26</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
       </c>
+      <c r="H9" t="n">
+        <v>82.88</v>
+      </c>
+      <c r="I9" t="n">
+        <v>88.15000000000002</v>
+      </c>
+      <c r="J9" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -19369,14 +20763,23 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>11.27</v>
+        <v>10.53</v>
       </c>
       <c r="F10" t="n">
-        <v>5.63</v>
+        <v>5.26</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
       </c>
+      <c r="H10" t="n">
+        <v>93.41</v>
+      </c>
+      <c r="I10" t="n">
+        <v>93.41000000000003</v>
+      </c>
+      <c r="J10" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -19385,7 +20788,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C11" t="n">
         <v>5</v>
@@ -19394,13 +20797,844 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>4.23</v>
+        <v>6.58</v>
       </c>
       <c r="F11" t="n">
-        <v>7.04</v>
+        <v>6.58</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>99.98999999999999</v>
+      </c>
+      <c r="I11" t="n">
+        <v>99.99000000000002</v>
+      </c>
+      <c r="J11" t="n">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Replication</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>URC</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>URC Mod</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>URC Percentage</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>URC Mod Percentage</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Baseline Percentage</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>URC Cum. Percentage</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>URC Mod Cum. Percentage</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Baseline Cum. Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" t="n">
+        <v>58</v>
+      </c>
+      <c r="D2" t="n">
+        <v>76</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5.26</v>
+      </c>
+      <c r="F2" t="n">
+        <v>76.31999999999999</v>
+      </c>
+      <c r="G2" t="n">
+        <v>100</v>
+      </c>
+      <c r="H2" t="n">
+        <v>5.26</v>
+      </c>
+      <c r="I2" t="n">
+        <v>76.31999999999999</v>
+      </c>
+      <c r="J2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>9</v>
+      </c>
+      <c r="C3" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>11.84</v>
+      </c>
+      <c r="F3" t="n">
+        <v>7.89</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>17.1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>84.20999999999999</v>
+      </c>
+      <c r="J3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>9</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>11.84</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3.95</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>28.94</v>
+      </c>
+      <c r="I4" t="n">
+        <v>88.16</v>
+      </c>
+      <c r="J4" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>8</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>10.53</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3.95</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>39.47</v>
+      </c>
+      <c r="I5" t="n">
+        <v>92.11</v>
+      </c>
+      <c r="J5" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>7</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>9.210000000000001</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3.95</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>48.68</v>
+      </c>
+      <c r="I6" t="n">
+        <v>96.06</v>
+      </c>
+      <c r="J6" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3.95</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2.63</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>52.63</v>
+      </c>
+      <c r="I7" t="n">
+        <v>98.69</v>
+      </c>
+      <c r="J7" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>10</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>13.16</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>65.79000000000001</v>
+      </c>
+      <c r="I8" t="n">
+        <v>98.69</v>
+      </c>
+      <c r="J8" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>9</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>11.84</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>77.63000000000001</v>
+      </c>
+      <c r="I9" t="n">
+        <v>98.69</v>
+      </c>
+      <c r="J9" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>11</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>14.47</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>92.10000000000001</v>
+      </c>
+      <c r="I10" t="n">
+        <v>100.01</v>
+      </c>
+      <c r="J10" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>6</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>7.89</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>99.99000000000001</v>
+      </c>
+      <c r="I11" t="n">
+        <v>100.01</v>
+      </c>
+      <c r="J11" t="n">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Replication</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>URC</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>URC Mod</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>URC Percentage</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>URC Mod Percentage</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Baseline Percentage</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>URC Cum. Percentage</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>URC Mod Cum. Percentage</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Baseline Cum. Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C2" t="n">
+        <v>61</v>
+      </c>
+      <c r="D2" t="n">
+        <v>76</v>
+      </c>
+      <c r="E2" t="n">
+        <v>7.89</v>
+      </c>
+      <c r="F2" t="n">
+        <v>80.26000000000001</v>
+      </c>
+      <c r="G2" t="n">
+        <v>100</v>
+      </c>
+      <c r="H2" t="n">
+        <v>7.89</v>
+      </c>
+      <c r="I2" t="n">
+        <v>80.26000000000001</v>
+      </c>
+      <c r="J2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>11</v>
+      </c>
+      <c r="C3" t="n">
+        <v>7</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>14.47</v>
+      </c>
+      <c r="F3" t="n">
+        <v>9.210000000000001</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>22.36</v>
+      </c>
+      <c r="I3" t="n">
+        <v>89.47</v>
+      </c>
+      <c r="J3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>10</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>13.16</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2.63</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>35.52</v>
+      </c>
+      <c r="I4" t="n">
+        <v>92.09999999999999</v>
+      </c>
+      <c r="J4" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>6</v>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>7.89</v>
+      </c>
+      <c r="F5" t="n">
+        <v>5.26</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>43.41</v>
+      </c>
+      <c r="I5" t="n">
+        <v>97.36</v>
+      </c>
+      <c r="J5" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>8</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>10.53</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>53.94</v>
+      </c>
+      <c r="I6" t="n">
+        <v>97.36</v>
+      </c>
+      <c r="J6" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2.63</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>56.57</v>
+      </c>
+      <c r="I7" t="n">
+        <v>98.67999999999999</v>
+      </c>
+      <c r="J7" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>8</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>10.53</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>67.09999999999999</v>
+      </c>
+      <c r="I8" t="n">
+        <v>99.99999999999999</v>
+      </c>
+      <c r="J8" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>11</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>14.47</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>81.56999999999999</v>
+      </c>
+      <c r="I9" t="n">
+        <v>99.99999999999999</v>
+      </c>
+      <c r="J9" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>10</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>13.16</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>94.72999999999999</v>
+      </c>
+      <c r="I10" t="n">
+        <v>99.99999999999999</v>
+      </c>
+      <c r="J10" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>5.26</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>99.98999999999999</v>
+      </c>
+      <c r="I11" t="n">
+        <v>99.99999999999999</v>
+      </c>
+      <c r="J11" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>